<commit_message>
Single Exam e2e workflow done
</commit_message>
<xml_diff>
--- a/scripts/Question_Breakup.xlsx
+++ b/scripts/Question_Breakup.xlsx
@@ -1,23 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="26812"/>
   <workbookPr filterPrivacy="1"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shaunakdas2020/Documents/workspace/ResoSapr/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shaunakdas2020/Documents/workspace/reso_marks/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27320" windowHeight="15360"/>
+    <workbookView xWindow="60" yWindow="460" windowWidth="27320" windowHeight="13540" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="IAT-1" sheetId="2" r:id="rId1"/>
+    <sheet name="IAT-1" sheetId="2" r:id="rId5"/>
+    <sheet name="IAT-2" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'IAT-1'!$A$1:$E$81</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'IAT-2'!$A$1:$E$81</definedName>
   </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="false"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="68" count="68">
   <si>
     <t>Question Number</t>
   </si>
@@ -150,31 +152,112 @@
   </si>
   <si>
     <t>A</t>
+  </si>
+  <si>
+    <t>projectile</t>
+  </si>
+  <si>
+    <t>Diversity</t>
+  </si>
+  <si>
+    <t>Co-ordinate geometry</t>
+  </si>
+  <si>
+    <t>Topics</t>
+  </si>
+  <si>
+    <t>Weightage in NSEJS</t>
+  </si>
+  <si>
+    <t>Normalised</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Difficulty Level </t>
+  </si>
+  <si>
+    <t>Maths</t>
+  </si>
+  <si>
+    <t>Carbon and It's compoound</t>
+  </si>
+  <si>
+    <t>Bio</t>
+  </si>
+  <si>
+    <t>lines and Angles</t>
+  </si>
+  <si>
+    <t>NLM</t>
+  </si>
+  <si>
+    <t>Polynomial</t>
+  </si>
+  <si>
+    <t>Chem</t>
+  </si>
+  <si>
+    <t>Excretion</t>
+  </si>
+  <si>
+    <t>Matter</t>
+  </si>
+  <si>
+    <t>Phy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cell </t>
+  </si>
+  <si>
+    <t>Please check sir some error</t>
+  </si>
+  <si>
+    <t>Work,Power energy</t>
+  </si>
+  <si>
+    <t>Mole concept</t>
+  </si>
+  <si>
+    <t>Circular Motion</t>
+  </si>
+  <si>
+    <t>St. of Atom</t>
+  </si>
+  <si>
+    <t>Metals and non Metals</t>
+  </si>
+  <si>
+    <t>Acid, Base and Salt</t>
+  </si>
+  <si>
+    <t>Motion</t>
+  </si>
+  <si>
+    <t>cell division</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]General"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="11"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -187,8 +270,38 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -224,12 +337,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -278,13 +400,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Excel Built-in Normal" xfId="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <tableStyles defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9" count="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -458,7 +615,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
+          <a:lin ang="16200000" scaled="false"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -487,7 +644,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="false">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -496,7 +653,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="false">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -505,7 +662,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="false">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -582,15 +739,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R81"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
+  <dimension ref="A1:M81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="22.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.33203125" customWidth="1"/>
@@ -604,7 +761,7 @@
     <col min="18" max="18" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" customFormat="false" ht="30" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -636,7 +793,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" customFormat="false" ht="30" customHeight="1">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -666,7 +823,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" customFormat="false" ht="30" customHeight="1">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -696,7 +853,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" customFormat="false" ht="30" customHeight="1">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -726,7 +883,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" customFormat="false" ht="30" customHeight="1">
       <c r="A5" s="6">
         <v>4</v>
       </c>
@@ -756,7 +913,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" customFormat="false" ht="30" customHeight="1">
       <c r="A6" s="6">
         <v>5</v>
       </c>
@@ -787,7 +944,7 @@
       </c>
       <c r="M6" s="18"/>
     </row>
-    <row r="7" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" customFormat="false" ht="30" customHeight="1">
       <c r="A7" s="6">
         <v>6</v>
       </c>
@@ -818,7 +975,7 @@
       </c>
       <c r="M7" s="18"/>
     </row>
-    <row r="8" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" customFormat="false" ht="30" customHeight="1">
       <c r="A8" s="6">
         <v>7</v>
       </c>
@@ -849,7 +1006,7 @@
       </c>
       <c r="M8" s="18"/>
     </row>
-    <row r="9" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" customFormat="false" ht="30" customHeight="1">
       <c r="A9" s="6">
         <v>8</v>
       </c>
@@ -880,7 +1037,7 @@
       </c>
       <c r="M9" s="18"/>
     </row>
-    <row r="10" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" customFormat="false" ht="30" customHeight="1">
       <c r="A10" s="6">
         <v>9</v>
       </c>
@@ -911,7 +1068,7 @@
       </c>
       <c r="M10" s="18"/>
     </row>
-    <row r="11" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" customFormat="false" ht="30" customHeight="1">
       <c r="A11" s="6">
         <v>10</v>
       </c>
@@ -942,7 +1099,7 @@
       </c>
       <c r="M11" s="18"/>
     </row>
-    <row r="12" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" customFormat="false" ht="30" customHeight="1">
       <c r="A12" s="6">
         <v>11</v>
       </c>
@@ -973,7 +1130,7 @@
       </c>
       <c r="M12" s="18"/>
     </row>
-    <row r="13" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" customFormat="false" ht="30" customHeight="1">
       <c r="A13" s="6">
         <v>12</v>
       </c>
@@ -1004,7 +1161,7 @@
       </c>
       <c r="M13" s="18"/>
     </row>
-    <row r="14" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" customFormat="false" ht="30" customHeight="1">
       <c r="A14" s="6">
         <v>13</v>
       </c>
@@ -1035,7 +1192,7 @@
       </c>
       <c r="M14" s="18"/>
     </row>
-    <row r="15" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" customFormat="false" ht="30" customHeight="1">
       <c r="A15" s="6">
         <v>14</v>
       </c>
@@ -1066,7 +1223,7 @@
       </c>
       <c r="M15" s="18"/>
     </row>
-    <row r="16" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" customFormat="false" ht="30" customHeight="1">
       <c r="A16" s="6">
         <v>15</v>
       </c>
@@ -1097,7 +1254,7 @@
       </c>
       <c r="M16" s="18"/>
     </row>
-    <row r="17" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" customFormat="false" ht="30" customHeight="1">
       <c r="A17" s="6">
         <v>16</v>
       </c>
@@ -1128,7 +1285,7 @@
       </c>
       <c r="M17" s="18"/>
     </row>
-    <row r="18" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" customFormat="false" ht="30" customHeight="1">
       <c r="A18" s="6">
         <v>17</v>
       </c>
@@ -1159,7 +1316,7 @@
       </c>
       <c r="M18" s="19"/>
     </row>
-    <row r="19" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" customFormat="false" ht="30" customHeight="1">
       <c r="A19" s="6">
         <v>18</v>
       </c>
@@ -1190,7 +1347,7 @@
       </c>
       <c r="M19" s="19"/>
     </row>
-    <row r="20" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" customFormat="false" ht="30" customHeight="1">
       <c r="A20" s="6">
         <v>19</v>
       </c>
@@ -1221,7 +1378,7 @@
       </c>
       <c r="M20" s="19"/>
     </row>
-    <row r="21" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" customFormat="false" ht="30" customHeight="1">
       <c r="A21" s="6">
         <v>20</v>
       </c>
@@ -1252,7 +1409,7 @@
       </c>
       <c r="M21" s="19"/>
     </row>
-    <row r="22" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" customFormat="false" ht="30" customHeight="1">
       <c r="A22" s="6">
         <v>21</v>
       </c>
@@ -1283,7 +1440,7 @@
       </c>
       <c r="M22" s="19"/>
     </row>
-    <row r="23" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" customFormat="false" ht="30" customHeight="1">
       <c r="A23" s="6">
         <v>22</v>
       </c>
@@ -1314,7 +1471,7 @@
       </c>
       <c r="M23" s="19"/>
     </row>
-    <row r="24" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" customFormat="false" ht="30" customHeight="1">
       <c r="A24" s="6">
         <v>23</v>
       </c>
@@ -1346,7 +1503,7 @@
       <c r="K24" s="20"/>
       <c r="M24" s="19"/>
     </row>
-    <row r="25" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" customFormat="false" ht="30" customHeight="1">
       <c r="A25" s="6">
         <v>24</v>
       </c>
@@ -1377,7 +1534,7 @@
       </c>
       <c r="M25" s="21"/>
     </row>
-    <row r="26" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" customFormat="false" ht="30" customHeight="1">
       <c r="A26" s="6">
         <v>25</v>
       </c>
@@ -1408,7 +1565,7 @@
       </c>
       <c r="M26" s="21"/>
     </row>
-    <row r="27" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" customFormat="false" ht="30" customHeight="1">
       <c r="A27" s="6">
         <v>26</v>
       </c>
@@ -1438,7 +1595,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" customFormat="false" ht="30" customHeight="1">
       <c r="A28" s="6">
         <v>27</v>
       </c>
@@ -1468,7 +1625,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" customFormat="false" ht="30" customHeight="1">
       <c r="A29" s="6">
         <v>28</v>
       </c>
@@ -1498,7 +1655,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" customFormat="false" ht="30" customHeight="1">
       <c r="A30" s="6">
         <v>29</v>
       </c>
@@ -1528,7 +1685,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" customFormat="false" ht="30" customHeight="1">
       <c r="A31" s="6">
         <v>30</v>
       </c>
@@ -1558,7 +1715,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" customFormat="false" ht="30" customHeight="1">
       <c r="A32" s="6">
         <v>31</v>
       </c>
@@ -1588,7 +1745,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" customFormat="false" ht="30" customHeight="1">
       <c r="A33" s="6">
         <v>32</v>
       </c>
@@ -1618,7 +1775,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" customFormat="false" ht="30" customHeight="1">
       <c r="A34" s="6">
         <v>33</v>
       </c>
@@ -1648,7 +1805,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" customFormat="false" ht="30" customHeight="1">
       <c r="A35" s="6">
         <v>34</v>
       </c>
@@ -1678,7 +1835,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" customFormat="false" ht="30" customHeight="1">
       <c r="A36" s="6">
         <v>35</v>
       </c>
@@ -1708,7 +1865,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" customFormat="false" ht="30" customHeight="1">
       <c r="A37" s="6">
         <v>36</v>
       </c>
@@ -1738,7 +1895,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10" customFormat="false" ht="30" customHeight="1">
       <c r="A38" s="6">
         <v>37</v>
       </c>
@@ -1768,7 +1925,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" customFormat="false" ht="30" customHeight="1">
       <c r="A39" s="6">
         <v>38</v>
       </c>
@@ -1798,7 +1955,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" customFormat="false" ht="30" customHeight="1">
       <c r="A40" s="6">
         <v>39</v>
       </c>
@@ -1828,7 +1985,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10" customFormat="false" ht="30" customHeight="1">
       <c r="A41" s="6">
         <v>40</v>
       </c>
@@ -1858,7 +2015,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10" customFormat="false" ht="30" customHeight="1">
       <c r="A42" s="6">
         <v>41</v>
       </c>
@@ -1888,7 +2045,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10" customFormat="false" ht="30" customHeight="1">
       <c r="A43" s="6">
         <v>42</v>
       </c>
@@ -1918,7 +2075,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10" customFormat="false" ht="30" customHeight="1">
       <c r="A44" s="6">
         <v>43</v>
       </c>
@@ -1948,7 +2105,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10" customFormat="false" ht="30" customHeight="1">
       <c r="A45" s="6">
         <v>44</v>
       </c>
@@ -1978,7 +2135,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:10" customFormat="false" ht="30" customHeight="1">
       <c r="A46" s="6">
         <v>45</v>
       </c>
@@ -2008,7 +2165,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:10" customFormat="false" ht="30" customHeight="1">
       <c r="A47" s="6">
         <v>46</v>
       </c>
@@ -2038,7 +2195,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:10" customFormat="false" ht="30" customHeight="1">
       <c r="A48" s="6">
         <v>47</v>
       </c>
@@ -2068,7 +2225,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="49" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:10" customFormat="false" ht="30" customHeight="1">
       <c r="A49" s="6">
         <v>48</v>
       </c>
@@ -2098,7 +2255,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="50" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:10" customFormat="false" ht="30" customHeight="1">
       <c r="A50" s="6">
         <v>49</v>
       </c>
@@ -2128,7 +2285,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:10" customFormat="false" ht="30" customHeight="1">
       <c r="A51" s="6">
         <v>50</v>
       </c>
@@ -2158,7 +2315,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="52" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:10" customFormat="false" ht="30" customHeight="1">
       <c r="A52" s="6">
         <v>51</v>
       </c>
@@ -2188,7 +2345,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:10" customFormat="false" ht="30" customHeight="1">
       <c r="A53" s="6">
         <v>52</v>
       </c>
@@ -2218,7 +2375,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="54" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:10" customFormat="false" ht="30" customHeight="1">
       <c r="A54" s="6">
         <v>53</v>
       </c>
@@ -2248,7 +2405,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="55" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:10" customFormat="false" ht="30" customHeight="1">
       <c r="A55" s="6">
         <v>54</v>
       </c>
@@ -2278,7 +2435,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:10" customFormat="false" ht="30" customHeight="1">
       <c r="A56" s="6">
         <v>55</v>
       </c>
@@ -2308,7 +2465,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="57" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:10" customFormat="false" ht="30" customHeight="1">
       <c r="A57" s="6">
         <v>56</v>
       </c>
@@ -2338,7 +2495,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="58" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:10" customFormat="false" ht="30" customHeight="1">
       <c r="A58" s="6">
         <v>57</v>
       </c>
@@ -2368,7 +2525,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="59" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:10" customFormat="false" ht="30" customHeight="1">
       <c r="A59" s="6">
         <v>58</v>
       </c>
@@ -2398,7 +2555,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="60" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:10" customFormat="false" ht="30" customHeight="1">
       <c r="A60" s="6">
         <v>59</v>
       </c>
@@ -2428,7 +2585,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="61" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:10" customFormat="false" ht="30" customHeight="1">
       <c r="A61" s="6">
         <v>60</v>
       </c>
@@ -2458,7 +2615,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="62" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:10" customFormat="false" ht="30" customHeight="1">
       <c r="A62" s="6">
         <v>61</v>
       </c>
@@ -2488,7 +2645,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="63" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:10" customFormat="false" ht="30" customHeight="1">
       <c r="A63" s="6">
         <v>62</v>
       </c>
@@ -2518,7 +2675,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:10" customFormat="false" ht="30" customHeight="1">
       <c r="A64" s="6">
         <v>63</v>
       </c>
@@ -2548,7 +2705,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="65" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:10" customFormat="false" ht="30" customHeight="1">
       <c r="A65" s="6">
         <v>64</v>
       </c>
@@ -2578,7 +2735,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="66" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:10" customFormat="false" ht="30" customHeight="1">
       <c r="A66" s="6">
         <v>65</v>
       </c>
@@ -2608,7 +2765,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="67" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:10" customFormat="false" ht="30" customHeight="1">
       <c r="A67" s="6">
         <v>66</v>
       </c>
@@ -2638,7 +2795,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="68" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:10" customFormat="false" ht="30" customHeight="1">
       <c r="A68" s="6">
         <v>67</v>
       </c>
@@ -2668,7 +2825,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="69" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:10" customFormat="false" ht="30" customHeight="1">
       <c r="A69" s="6">
         <v>68</v>
       </c>
@@ -2698,7 +2855,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="70" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:10" customFormat="false" ht="30" customHeight="1">
       <c r="A70" s="6">
         <v>69</v>
       </c>
@@ -2728,7 +2885,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="71" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:10" customFormat="false" ht="30" customHeight="1">
       <c r="A71" s="6">
         <v>70</v>
       </c>
@@ -2758,7 +2915,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="72" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:10" customFormat="false" ht="30" customHeight="1">
       <c r="A72" s="6">
         <v>71</v>
       </c>
@@ -2788,7 +2945,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="73" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:10" customFormat="false" ht="30" customHeight="1">
       <c r="A73" s="6">
         <v>72</v>
       </c>
@@ -2818,7 +2975,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="74" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:10" customFormat="false" ht="30" customHeight="1">
       <c r="A74" s="6">
         <v>73</v>
       </c>
@@ -2848,7 +3005,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="75" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:10" customFormat="false" ht="30" customHeight="1">
       <c r="A75" s="6">
         <v>74</v>
       </c>
@@ -2878,7 +3035,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="76" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:10" customFormat="false" ht="30" customHeight="1">
       <c r="A76" s="6">
         <v>75</v>
       </c>
@@ -2908,7 +3065,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="77" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:10" customFormat="false" ht="30" customHeight="1">
       <c r="A77" s="6">
         <v>76</v>
       </c>
@@ -2938,7 +3095,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="78" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:10" customFormat="false" ht="30" customHeight="1">
       <c r="A78" s="6">
         <v>77</v>
       </c>
@@ -2968,7 +3125,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="79" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:10" customFormat="false" ht="30" customHeight="1">
       <c r="A79" s="6">
         <v>78</v>
       </c>
@@ -2998,7 +3155,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="80" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:10" customFormat="false" ht="30" customHeight="1">
       <c r="A80" s="6">
         <v>79</v>
       </c>
@@ -3028,7 +3185,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="81" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:10" customFormat="false" ht="30" customHeight="1">
       <c r="A81" s="6">
         <v>80</v>
       </c>
@@ -3056,6 +3213,2800 @@
       <c r="I81" s="11"/>
       <c r="J81" t="s">
         <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="M25:M26"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
+  <dimension ref="A1:R81"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" customWidth="1"/>
+    <col min="3" max="4" width="31.6640625" customWidth="1"/>
+    <col min="5" max="10" width="18.83203125" customWidth="1"/>
+    <col min="11" max="11" width="31.6640625" customWidth="1"/>
+    <col min="12" max="12" width="18.5" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="16" width="24.5" customWidth="1"/>
+    <col min="17" max="17" width="30.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" customFormat="false" ht="30" customHeight="1">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="L1" s="2"/>
+    </row>
+    <row r="2" spans="1:10" customFormat="false" ht="30" customHeight="1">
+      <c r="A2" s="6">
+        <v>1</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="16">
+        <v>3</v>
+      </c>
+      <c r="G2" s="16">
+        <v>-1</v>
+      </c>
+      <c r="H2" s="16">
+        <v>0</v>
+      </c>
+      <c r="I2" s="16"/>
+      <c r="J2" s="0" t="str">
+        <v>D</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" customFormat="false" ht="30" customHeight="1">
+      <c r="A3" s="6">
+        <v>2</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="16">
+        <v>3</v>
+      </c>
+      <c r="G3" s="16">
+        <v>-1</v>
+      </c>
+      <c r="H3" s="16">
+        <v>0</v>
+      </c>
+      <c r="I3" s="16"/>
+      <c r="J3" s="0" t="str">
+        <v>C</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" customFormat="false" ht="30" customHeight="1">
+      <c r="A4" s="6">
+        <v>3</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="16">
+        <v>3</v>
+      </c>
+      <c r="G4" s="16">
+        <v>-1</v>
+      </c>
+      <c r="H4" s="16">
+        <v>0</v>
+      </c>
+      <c r="I4" s="16"/>
+      <c r="J4" s="0" t="str">
+        <v>D</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" customFormat="false" ht="30" customHeight="1">
+      <c r="A5" s="6">
+        <v>4</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="16">
+        <v>3</v>
+      </c>
+      <c r="G5" s="16">
+        <v>-1</v>
+      </c>
+      <c r="H5" s="16">
+        <v>0</v>
+      </c>
+      <c r="I5" s="12"/>
+      <c r="J5" s="0" t="str">
+        <v>A</v>
+      </c>
+      <c r="K5" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="L5" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="M5" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="O5" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="P5" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q5" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="R5" s="24" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" customFormat="false" ht="30" customHeight="1">
+      <c r="A6" s="6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="16">
+        <v>3</v>
+      </c>
+      <c r="G6" s="16">
+        <v>-1</v>
+      </c>
+      <c r="H6" s="16">
+        <v>0</v>
+      </c>
+      <c r="I6" s="12"/>
+      <c r="J6" s="0" t="str">
+        <v>D</v>
+      </c>
+      <c r="K6" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="L6" s="26">
+        <v>22</v>
+      </c>
+      <c r="M6" s="27">
+        <f>L6/26*20</f>
+        <v>16.923076923076923</v>
+      </c>
+      <c r="N6" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="O6" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="P6" s="24">
+        <f>COUNTIFS($B:$B,$O6,$E:$E,P$5)</f>
+        <v>5</v>
+      </c>
+      <c r="Q6" s="24">
+        <f>COUNTIFS($B:$B,$O6,$E:$E,Q$5)</f>
+        <v>8</v>
+      </c>
+      <c r="R6" s="24">
+        <f>COUNTIFS($B:$B,$O6,$E:$E,R$5)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" customFormat="false" ht="30" customHeight="1">
+      <c r="A7" s="6">
+        <v>6</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="16">
+        <v>3</v>
+      </c>
+      <c r="G7" s="16">
+        <v>-1</v>
+      </c>
+      <c r="H7" s="16">
+        <v>0</v>
+      </c>
+      <c r="I7" s="12"/>
+      <c r="J7" s="0" t="str">
+        <v>D</v>
+      </c>
+      <c r="K7" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="L7" s="26">
+        <v>4</v>
+      </c>
+      <c r="M7" s="27">
+        <f>L7/26*20</f>
+        <v>3.0769230769230771</v>
+      </c>
+      <c r="N7" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="O7" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="P7" s="24">
+        <f>COUNTIFS($B:$B,$O7,$E:$E,P$5)</f>
+        <v>9</v>
+      </c>
+      <c r="Q7" s="24">
+        <f>COUNTIFS($B:$B,$O7,$E:$E,Q$5)</f>
+        <v>5</v>
+      </c>
+      <c r="R7" s="24">
+        <f>COUNTIFS($B:$B,$O7,$E:$E,R$5)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" customFormat="false" ht="30" customHeight="1">
+      <c r="A8" s="6">
+        <v>7</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="16">
+        <v>3</v>
+      </c>
+      <c r="G8" s="16">
+        <v>-1</v>
+      </c>
+      <c r="H8" s="16">
+        <v>0</v>
+      </c>
+      <c r="I8" s="12"/>
+      <c r="J8" s="0" t="str">
+        <v>C</v>
+      </c>
+      <c r="K8" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="L8" s="30">
+        <v>15</v>
+      </c>
+      <c r="M8" s="31">
+        <f>L8*20/31</f>
+        <v>9.67741935483871</v>
+      </c>
+      <c r="N8" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="O8" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="P8" s="24">
+        <f>COUNTIFS($B:$B,$O8,$E:$E,P$5)</f>
+        <v>6</v>
+      </c>
+      <c r="Q8" s="24">
+        <f>COUNTIFS($B:$B,$O8,$E:$E,Q$5)</f>
+        <v>4</v>
+      </c>
+      <c r="R8" s="24">
+        <f>COUNTIFS($B:$B,$O8,$E:$E,R$5)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" customFormat="false" ht="30" customHeight="1">
+      <c r="A9" s="6">
+        <v>8</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="16">
+        <v>3</v>
+      </c>
+      <c r="G9" s="16">
+        <v>-1</v>
+      </c>
+      <c r="H9" s="16">
+        <v>0</v>
+      </c>
+      <c r="I9" s="12"/>
+      <c r="J9" s="0" t="str">
+        <v>B</v>
+      </c>
+      <c r="K9" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="L9" s="30">
+        <v>5</v>
+      </c>
+      <c r="M9" s="31">
+        <f t="shared" ref="M9:M12" si="0">L9*20/31</f>
+        <v>3.225806451612903</v>
+      </c>
+      <c r="N9" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="O9" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="P9" s="24">
+        <f>COUNTIFS($B:$B,$O9,$E:$E,P$5)</f>
+        <v>5</v>
+      </c>
+      <c r="Q9" s="24">
+        <f>COUNTIFS($B:$B,$O9,$E:$E,Q$5)</f>
+        <v>10</v>
+      </c>
+      <c r="R9" s="24">
+        <f>COUNTIFS($B:$B,$O9,$E:$E,R$5)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" customFormat="false" ht="30" customHeight="1">
+      <c r="A10" s="6">
+        <v>9</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="16">
+        <v>3</v>
+      </c>
+      <c r="G10" s="16">
+        <v>-1</v>
+      </c>
+      <c r="H10" s="16">
+        <v>0</v>
+      </c>
+      <c r="I10" s="12"/>
+      <c r="J10" s="0" t="str">
+        <v>C</v>
+      </c>
+      <c r="K10" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="L10" s="30">
+        <v>2</v>
+      </c>
+      <c r="M10" s="31">
+        <f t="shared" si="0"/>
+        <v>1.2903225806451613</v>
+      </c>
+      <c r="N10" s="32" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" customFormat="false" ht="30" customHeight="1">
+      <c r="A11" s="6">
+        <v>10</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="16">
+        <v>3</v>
+      </c>
+      <c r="G11" s="16">
+        <v>-1</v>
+      </c>
+      <c r="H11" s="16">
+        <v>0</v>
+      </c>
+      <c r="I11" s="12"/>
+      <c r="J11" s="0" t="str">
+        <v>C</v>
+      </c>
+      <c r="K11" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="L11" s="30">
+        <v>5</v>
+      </c>
+      <c r="M11" s="31">
+        <f t="shared" si="0"/>
+        <v>3.225806451612903</v>
+      </c>
+      <c r="N11" s="32" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" customFormat="false" ht="30" customHeight="1">
+      <c r="A12" s="6">
+        <v>11</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="16">
+        <v>3</v>
+      </c>
+      <c r="G12" s="16">
+        <v>-1</v>
+      </c>
+      <c r="H12" s="16">
+        <v>0</v>
+      </c>
+      <c r="I12" s="12"/>
+      <c r="J12" s="0" t="str">
+        <v>A</v>
+      </c>
+      <c r="K12" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="L12" s="30">
+        <v>4</v>
+      </c>
+      <c r="M12" s="31">
+        <f t="shared" si="0"/>
+        <v>2.5806451612903225</v>
+      </c>
+      <c r="N12" s="32" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" customFormat="false" ht="30" customHeight="1">
+      <c r="A13" s="6">
+        <v>12</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="16">
+        <v>3</v>
+      </c>
+      <c r="G13" s="16">
+        <v>-1</v>
+      </c>
+      <c r="H13" s="16">
+        <v>0</v>
+      </c>
+      <c r="I13" s="12"/>
+      <c r="J13" s="0" t="str">
+        <v>D</v>
+      </c>
+      <c r="K13" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="L13" s="34">
+        <v>8</v>
+      </c>
+      <c r="M13" s="35">
+        <f>L13*20/46</f>
+        <v>3.4782608695652173</v>
+      </c>
+      <c r="N13" s="36" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" customFormat="false" ht="30" customHeight="1">
+      <c r="A14" s="6">
+        <v>13</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="16">
+        <v>3</v>
+      </c>
+      <c r="G14" s="16">
+        <v>-1</v>
+      </c>
+      <c r="H14" s="16">
+        <v>0</v>
+      </c>
+      <c r="I14" s="12"/>
+      <c r="J14" s="0" t="str">
+        <v>A</v>
+      </c>
+      <c r="K14" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="L14" s="34">
+        <v>4</v>
+      </c>
+      <c r="M14" s="35">
+        <f t="shared" ref="M14:M17" si="1">L14*20/46</f>
+        <v>1.7391304347826086</v>
+      </c>
+      <c r="N14" s="36" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" customFormat="false" ht="30" customHeight="1">
+      <c r="A15" s="6">
+        <v>14</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="D15" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" s="16">
+        <v>3</v>
+      </c>
+      <c r="G15" s="16">
+        <v>-1</v>
+      </c>
+      <c r="H15" s="16">
+        <v>0</v>
+      </c>
+      <c r="I15" s="12"/>
+      <c r="J15" s="0" t="str">
+        <v>A</v>
+      </c>
+      <c r="K15" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="L15" s="34">
+        <v>18</v>
+      </c>
+      <c r="M15" s="35">
+        <f t="shared" si="1"/>
+        <v>7.8260869565217392</v>
+      </c>
+      <c r="N15" s="36" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" customFormat="false" ht="30" customHeight="1">
+      <c r="A16" s="6">
+        <v>15</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" s="16">
+        <v>3</v>
+      </c>
+      <c r="G16" s="16">
+        <v>-1</v>
+      </c>
+      <c r="H16" s="16">
+        <v>0</v>
+      </c>
+      <c r="I16" s="12"/>
+      <c r="J16" s="0" t="str">
+        <v>D</v>
+      </c>
+      <c r="K16" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="L16" s="34">
+        <v>4</v>
+      </c>
+      <c r="M16" s="35">
+        <f t="shared" si="1"/>
+        <v>1.7391304347826086</v>
+      </c>
+      <c r="N16" s="36" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" customFormat="false" ht="30" customHeight="1">
+      <c r="A17" s="6">
+        <v>16</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="16">
+        <v>3</v>
+      </c>
+      <c r="G17" s="16">
+        <v>-1</v>
+      </c>
+      <c r="H17" s="16">
+        <v>0</v>
+      </c>
+      <c r="I17" s="12"/>
+      <c r="J17" s="0" t="str">
+        <v>C</v>
+      </c>
+      <c r="K17" s="33" t="s">
+        <v>56</v>
+      </c>
+      <c r="L17" s="34">
+        <v>12</v>
+      </c>
+      <c r="M17" s="35">
+        <f t="shared" si="1"/>
+        <v>5.2173913043478262</v>
+      </c>
+      <c r="N17" s="36" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" customFormat="false" ht="30" customHeight="1">
+      <c r="A18" s="6">
+        <v>17</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="D18" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="E18" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" s="16">
+        <v>3</v>
+      </c>
+      <c r="G18" s="16">
+        <v>-1</v>
+      </c>
+      <c r="H18" s="16">
+        <v>0</v>
+      </c>
+      <c r="I18" s="12"/>
+      <c r="J18" s="0" t="str">
+        <v>B</v>
+      </c>
+      <c r="K18" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="L18" s="13">
+        <v>17</v>
+      </c>
+      <c r="M18" s="38">
+        <f>L18*20/50</f>
+        <v>6.8</v>
+      </c>
+      <c r="N18" s="39" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" customFormat="false" ht="30" customHeight="1">
+      <c r="A19" s="6">
+        <v>18</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="D19" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="E19" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F19" s="16">
+        <v>3</v>
+      </c>
+      <c r="G19" s="16">
+        <v>-1</v>
+      </c>
+      <c r="H19" s="16">
+        <v>0</v>
+      </c>
+      <c r="I19" s="16"/>
+      <c r="J19" s="0" t="str">
+        <v>C</v>
+      </c>
+      <c r="K19" s="40" t="s">
+        <v>8</v>
+      </c>
+      <c r="L19" s="40">
+        <v>2</v>
+      </c>
+      <c r="M19" s="38">
+        <f t="shared" ref="M19:M23" si="2">L19*20/50</f>
+        <v>0.8</v>
+      </c>
+      <c r="N19" s="39" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" customFormat="false" ht="30" customHeight="1">
+      <c r="A20" s="6">
+        <v>19</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="E20" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F20" s="16">
+        <v>3</v>
+      </c>
+      <c r="G20" s="16">
+        <v>-1</v>
+      </c>
+      <c r="H20" s="16">
+        <v>0</v>
+      </c>
+      <c r="I20" s="16"/>
+      <c r="J20" s="0" t="str">
+        <v>D</v>
+      </c>
+      <c r="K20" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="L20" s="40">
+        <v>2</v>
+      </c>
+      <c r="M20" s="38">
+        <f t="shared" si="2"/>
+        <v>0.8</v>
+      </c>
+      <c r="N20" s="39" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" customFormat="false" ht="30" customHeight="1">
+      <c r="A21" s="6">
+        <v>20</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="D21" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="E21" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F21" s="16">
+        <v>3</v>
+      </c>
+      <c r="G21" s="16">
+        <v>-1</v>
+      </c>
+      <c r="H21" s="16">
+        <v>0</v>
+      </c>
+      <c r="I21" s="16"/>
+      <c r="J21" s="0" t="str">
+        <v>D</v>
+      </c>
+      <c r="K21" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="L21" s="40">
+        <v>7</v>
+      </c>
+      <c r="M21" s="38">
+        <f t="shared" si="2"/>
+        <v>2.8</v>
+      </c>
+      <c r="N21" s="39" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" customFormat="false" ht="30" customHeight="1">
+      <c r="A22" s="6">
+        <v>21</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="D22" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="E22" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F22" s="16">
+        <v>3</v>
+      </c>
+      <c r="G22" s="16">
+        <v>-1</v>
+      </c>
+      <c r="H22" s="16">
+        <v>0</v>
+      </c>
+      <c r="I22" s="16"/>
+      <c r="J22" s="0" t="str">
+        <v>C</v>
+      </c>
+      <c r="K22" s="40" t="s">
+        <v>27</v>
+      </c>
+      <c r="L22" s="24">
+        <v>10</v>
+      </c>
+      <c r="M22" s="38">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="N22" s="39" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" customFormat="false" ht="30" customHeight="1">
+      <c r="A23" s="6">
+        <v>22</v>
+      </c>
+      <c r="B23" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="D23" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="E23" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F23" s="16">
+        <v>3</v>
+      </c>
+      <c r="G23" s="16">
+        <v>-1</v>
+      </c>
+      <c r="H23" s="16">
+        <v>0</v>
+      </c>
+      <c r="I23" s="16"/>
+      <c r="J23" s="0" t="str">
+        <v>A</v>
+      </c>
+      <c r="K23" s="40" t="s">
+        <v>28</v>
+      </c>
+      <c r="L23" s="40">
+        <v>5</v>
+      </c>
+      <c r="M23" s="38">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="N23" s="39" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" customFormat="false" ht="30" customHeight="1">
+      <c r="A24" s="6">
+        <v>23</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F24" s="16">
+        <v>3</v>
+      </c>
+      <c r="G24" s="16">
+        <v>-1</v>
+      </c>
+      <c r="H24" s="16">
+        <v>0</v>
+      </c>
+      <c r="I24" s="16"/>
+      <c r="J24" s="0" t="str">
+        <v>A</v>
+      </c>
+      <c r="K24" s="41" t="s">
+        <v>29</v>
+      </c>
+      <c r="L24" s="42">
+        <v>7</v>
+      </c>
+      <c r="M24" s="43">
+        <v>3</v>
+      </c>
+      <c r="N24" s="44" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" customFormat="false" ht="30" customHeight="1">
+      <c r="A25" s="6">
+        <v>24</v>
+      </c>
+      <c r="B25" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="D25" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="E25" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F25" s="16">
+        <v>3</v>
+      </c>
+      <c r="G25" s="16">
+        <v>-1</v>
+      </c>
+      <c r="H25" s="16">
+        <v>0</v>
+      </c>
+      <c r="I25" s="11"/>
+      <c r="J25" s="0" t="str">
+        <v>BONUS</v>
+      </c>
+      <c r="M25" s="45" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" customFormat="false" ht="30" customHeight="1">
+      <c r="A26" s="6">
+        <v>25</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="D26" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="E26" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F26" s="16">
+        <v>3</v>
+      </c>
+      <c r="G26" s="16">
+        <v>-1</v>
+      </c>
+      <c r="H26" s="16">
+        <v>0</v>
+      </c>
+      <c r="I26" s="11"/>
+      <c r="J26" s="0" t="str">
+        <v>D</v>
+      </c>
+      <c r="M26" s="46"/>
+    </row>
+    <row r="27" spans="1:10" customFormat="false" ht="30" customHeight="1">
+      <c r="A27" s="6">
+        <v>26</v>
+      </c>
+      <c r="B27" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="D27" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="E27" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F27" s="16">
+        <v>3</v>
+      </c>
+      <c r="G27" s="16">
+        <v>-1</v>
+      </c>
+      <c r="H27" s="16">
+        <v>0</v>
+      </c>
+      <c r="I27" s="11"/>
+      <c r="J27" s="0" t="str">
+        <v>A</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" customFormat="false" ht="30" customHeight="1">
+      <c r="A28" s="6">
+        <v>27</v>
+      </c>
+      <c r="B28" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D28" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F28" s="16">
+        <v>3</v>
+      </c>
+      <c r="G28" s="16">
+        <v>-1</v>
+      </c>
+      <c r="H28" s="16">
+        <v>0</v>
+      </c>
+      <c r="I28" s="11"/>
+      <c r="J28" s="0" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" customFormat="false" ht="30" customHeight="1">
+      <c r="A29" s="6">
+        <v>28</v>
+      </c>
+      <c r="B29" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="D29" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="E29" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F29" s="16">
+        <v>3</v>
+      </c>
+      <c r="G29" s="16">
+        <v>-1</v>
+      </c>
+      <c r="H29" s="16">
+        <v>0</v>
+      </c>
+      <c r="I29" s="11"/>
+      <c r="J29" s="0" t="str">
+        <v>C</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" customFormat="false" ht="30" customHeight="1">
+      <c r="A30" s="6">
+        <v>29</v>
+      </c>
+      <c r="B30" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="D30" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="E30" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F30" s="16">
+        <v>3</v>
+      </c>
+      <c r="G30" s="16">
+        <v>-1</v>
+      </c>
+      <c r="H30" s="16">
+        <v>0</v>
+      </c>
+      <c r="I30" s="11"/>
+      <c r="J30" s="0" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" customFormat="false" ht="30" customHeight="1">
+      <c r="A31" s="6">
+        <v>30</v>
+      </c>
+      <c r="B31" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="D31" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="E31" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F31" s="16">
+        <v>3</v>
+      </c>
+      <c r="G31" s="16">
+        <v>-1</v>
+      </c>
+      <c r="H31" s="16">
+        <v>0</v>
+      </c>
+      <c r="I31" s="11"/>
+      <c r="J31" s="0" t="str">
+        <v>C</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" customFormat="false" ht="30" customHeight="1">
+      <c r="A32" s="6">
+        <v>31</v>
+      </c>
+      <c r="B32" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="D32" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="E32" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F32" s="16">
+        <v>3</v>
+      </c>
+      <c r="G32" s="16">
+        <v>-1</v>
+      </c>
+      <c r="H32" s="16">
+        <v>0</v>
+      </c>
+      <c r="I32" s="11"/>
+      <c r="J32" s="0" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" customFormat="false" ht="30" customHeight="1">
+      <c r="A33" s="6">
+        <v>32</v>
+      </c>
+      <c r="B33" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="D33" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="E33" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F33" s="16">
+        <v>3</v>
+      </c>
+      <c r="G33" s="16">
+        <v>-1</v>
+      </c>
+      <c r="H33" s="16">
+        <v>0</v>
+      </c>
+      <c r="I33" s="11"/>
+      <c r="J33" s="0" t="str">
+        <v>D</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" customFormat="false" ht="30" customHeight="1">
+      <c r="A34" s="6">
+        <v>33</v>
+      </c>
+      <c r="B34" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C34" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="D34" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="E34" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F34" s="16">
+        <v>3</v>
+      </c>
+      <c r="G34" s="16">
+        <v>-1</v>
+      </c>
+      <c r="H34" s="16">
+        <v>0</v>
+      </c>
+      <c r="I34" s="11"/>
+      <c r="J34" s="0" t="str">
+        <v>D</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" customFormat="false" ht="30" customHeight="1">
+      <c r="A35" s="6">
+        <v>34</v>
+      </c>
+      <c r="B35" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="D35" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="E35" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F35" s="16">
+        <v>3</v>
+      </c>
+      <c r="G35" s="16">
+        <v>-1</v>
+      </c>
+      <c r="H35" s="16">
+        <v>0</v>
+      </c>
+      <c r="I35" s="11"/>
+      <c r="J35" s="0" t="str">
+        <v>C</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" customFormat="false" ht="30" customHeight="1">
+      <c r="A36" s="6">
+        <v>35</v>
+      </c>
+      <c r="B36" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C36" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D36" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="E36" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F36" s="16">
+        <v>3</v>
+      </c>
+      <c r="G36" s="16">
+        <v>-1</v>
+      </c>
+      <c r="H36" s="16">
+        <v>0</v>
+      </c>
+      <c r="I36" s="11"/>
+      <c r="J36" s="0" t="str">
+        <v>A</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" customFormat="false" ht="30" customHeight="1">
+      <c r="A37" s="6">
+        <v>36</v>
+      </c>
+      <c r="B37" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C37" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="D37" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="E37" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F37" s="16">
+        <v>3</v>
+      </c>
+      <c r="G37" s="16">
+        <v>-1</v>
+      </c>
+      <c r="H37" s="16">
+        <v>0</v>
+      </c>
+      <c r="I37" s="11"/>
+      <c r="J37" s="0" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" customFormat="false" ht="30" customHeight="1">
+      <c r="A38" s="6">
+        <v>37</v>
+      </c>
+      <c r="B38" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C38" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D38" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="E38" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F38" s="16">
+        <v>3</v>
+      </c>
+      <c r="G38" s="16">
+        <v>-1</v>
+      </c>
+      <c r="H38" s="16">
+        <v>0</v>
+      </c>
+      <c r="I38" s="11"/>
+      <c r="J38" s="0" t="str">
+        <v>C</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" customFormat="false" ht="30" customHeight="1">
+      <c r="A39" s="6">
+        <v>38</v>
+      </c>
+      <c r="B39" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C39" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="D39" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="E39" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F39" s="16">
+        <v>3</v>
+      </c>
+      <c r="G39" s="16">
+        <v>-1</v>
+      </c>
+      <c r="H39" s="16">
+        <v>0</v>
+      </c>
+      <c r="I39" s="11"/>
+      <c r="J39" s="0" t="str">
+        <v>C</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" customFormat="false" ht="30" customHeight="1">
+      <c r="A40" s="6">
+        <v>39</v>
+      </c>
+      <c r="B40" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C40" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="D40" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="E40" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F40" s="16">
+        <v>3</v>
+      </c>
+      <c r="G40" s="16">
+        <v>-1</v>
+      </c>
+      <c r="H40" s="16">
+        <v>0</v>
+      </c>
+      <c r="I40" s="11"/>
+      <c r="J40" s="0" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" customFormat="false" ht="30" customHeight="1">
+      <c r="A41" s="6">
+        <v>40</v>
+      </c>
+      <c r="B41" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C41" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="D41" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="E41" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F41" s="16">
+        <v>3</v>
+      </c>
+      <c r="G41" s="16">
+        <v>-1</v>
+      </c>
+      <c r="H41" s="16">
+        <v>0</v>
+      </c>
+      <c r="I41" s="11"/>
+      <c r="J41" s="0" t="str">
+        <v>C</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" customFormat="false" ht="30" customHeight="1">
+      <c r="A42" s="6">
+        <v>41</v>
+      </c>
+      <c r="B42" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C42" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="D42" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="E42" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F42" s="16">
+        <v>3</v>
+      </c>
+      <c r="G42" s="16">
+        <v>-1</v>
+      </c>
+      <c r="H42" s="16">
+        <v>0</v>
+      </c>
+      <c r="I42" s="11"/>
+      <c r="J42" s="0" t="str">
+        <v>C</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" customFormat="false" ht="30" customHeight="1">
+      <c r="A43" s="6">
+        <v>42</v>
+      </c>
+      <c r="B43" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C43" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="D43" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="E43" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F43" s="16">
+        <v>3</v>
+      </c>
+      <c r="G43" s="16">
+        <v>-1</v>
+      </c>
+      <c r="H43" s="16">
+        <v>0</v>
+      </c>
+      <c r="I43" s="11"/>
+      <c r="J43" s="0" t="str">
+        <v>A</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" customFormat="false" ht="30" customHeight="1">
+      <c r="A44" s="6">
+        <v>43</v>
+      </c>
+      <c r="B44" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C44" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D44" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="E44" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F44" s="16">
+        <v>3</v>
+      </c>
+      <c r="G44" s="16">
+        <v>-1</v>
+      </c>
+      <c r="H44" s="16">
+        <v>0</v>
+      </c>
+      <c r="I44" s="11"/>
+      <c r="J44" s="0" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" customFormat="false" ht="30" customHeight="1">
+      <c r="A45" s="6">
+        <v>44</v>
+      </c>
+      <c r="B45" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C45" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="D45" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="E45" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F45" s="16">
+        <v>3</v>
+      </c>
+      <c r="G45" s="16">
+        <v>-1</v>
+      </c>
+      <c r="H45" s="16">
+        <v>0</v>
+      </c>
+      <c r="I45" s="11"/>
+      <c r="J45" s="0" t="str">
+        <v>C</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" customFormat="false" ht="30" customHeight="1">
+      <c r="A46" s="6">
+        <v>45</v>
+      </c>
+      <c r="B46" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C46" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D46" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="E46" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F46" s="16">
+        <v>3</v>
+      </c>
+      <c r="G46" s="16">
+        <v>-1</v>
+      </c>
+      <c r="H46" s="16">
+        <v>0</v>
+      </c>
+      <c r="I46" s="11"/>
+      <c r="J46" s="0" t="str">
+        <v>A</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" customFormat="false" ht="30" customHeight="1">
+      <c r="A47" s="6">
+        <v>46</v>
+      </c>
+      <c r="B47" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C47" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="D47" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="E47" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F47" s="16">
+        <v>3</v>
+      </c>
+      <c r="G47" s="16">
+        <v>-1</v>
+      </c>
+      <c r="H47" s="16">
+        <v>0</v>
+      </c>
+      <c r="I47" s="11"/>
+      <c r="J47" s="0" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" customFormat="false" ht="30" customHeight="1">
+      <c r="A48" s="6">
+        <v>47</v>
+      </c>
+      <c r="B48" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C48" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="D48" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="E48" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F48" s="16">
+        <v>3</v>
+      </c>
+      <c r="G48" s="16">
+        <v>-1</v>
+      </c>
+      <c r="H48" s="16">
+        <v>0</v>
+      </c>
+      <c r="I48" s="11"/>
+      <c r="J48" s="0" t="str">
+        <v>D</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" customFormat="false" ht="30" customHeight="1">
+      <c r="A49" s="6">
+        <v>48</v>
+      </c>
+      <c r="B49" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C49" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="D49" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="E49" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F49" s="16">
+        <v>3</v>
+      </c>
+      <c r="G49" s="16">
+        <v>-1</v>
+      </c>
+      <c r="H49" s="16">
+        <v>0</v>
+      </c>
+      <c r="I49" s="11"/>
+      <c r="J49" s="0" t="str">
+        <v>C</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" customFormat="false" ht="30" customHeight="1">
+      <c r="A50" s="6">
+        <v>49</v>
+      </c>
+      <c r="B50" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C50" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="D50" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="E50" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F50" s="16">
+        <v>3</v>
+      </c>
+      <c r="G50" s="16">
+        <v>-1</v>
+      </c>
+      <c r="H50" s="16">
+        <v>0</v>
+      </c>
+      <c r="I50" s="11"/>
+      <c r="J50" s="0" t="str">
+        <v>A</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" customFormat="false" ht="30" customHeight="1">
+      <c r="A51" s="6">
+        <v>50</v>
+      </c>
+      <c r="B51" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C51" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="D51" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="E51" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F51" s="16">
+        <v>3</v>
+      </c>
+      <c r="G51" s="16">
+        <v>-1</v>
+      </c>
+      <c r="H51" s="16">
+        <v>0</v>
+      </c>
+      <c r="I51" s="11"/>
+      <c r="J51" s="0" t="str">
+        <v>C</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" customFormat="false" ht="30" customHeight="1">
+      <c r="A52" s="6">
+        <v>51</v>
+      </c>
+      <c r="B52" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C52" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="D52" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="E52" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F52" s="16">
+        <v>3</v>
+      </c>
+      <c r="G52" s="16">
+        <v>-1</v>
+      </c>
+      <c r="H52" s="16">
+        <v>0</v>
+      </c>
+      <c r="I52" s="11"/>
+      <c r="J52" s="0" t="str">
+        <v>A</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" customFormat="false" ht="30" customHeight="1">
+      <c r="A53" s="6">
+        <v>52</v>
+      </c>
+      <c r="B53" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C53" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="D53" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="E53" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F53" s="16">
+        <v>3</v>
+      </c>
+      <c r="G53" s="16">
+        <v>-1</v>
+      </c>
+      <c r="H53" s="16">
+        <v>0</v>
+      </c>
+      <c r="I53" s="11"/>
+      <c r="J53" s="0" t="str">
+        <v>D</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" customFormat="false" ht="30" customHeight="1">
+      <c r="A54" s="6">
+        <v>53</v>
+      </c>
+      <c r="B54" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C54" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="D54" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="E54" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F54" s="16">
+        <v>3</v>
+      </c>
+      <c r="G54" s="16">
+        <v>-1</v>
+      </c>
+      <c r="H54" s="16">
+        <v>0</v>
+      </c>
+      <c r="I54" s="11"/>
+      <c r="J54" s="0" t="str">
+        <v>A</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" customFormat="false" ht="30" customHeight="1">
+      <c r="A55" s="6">
+        <v>54</v>
+      </c>
+      <c r="B55" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C55" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="D55" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="E55" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F55" s="16">
+        <v>3</v>
+      </c>
+      <c r="G55" s="16">
+        <v>-1</v>
+      </c>
+      <c r="H55" s="16">
+        <v>0</v>
+      </c>
+      <c r="I55" s="11"/>
+      <c r="J55" s="0" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" customFormat="false" ht="30" customHeight="1">
+      <c r="A56" s="6">
+        <v>55</v>
+      </c>
+      <c r="B56" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C56" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="D56" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="E56" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F56" s="16">
+        <v>3</v>
+      </c>
+      <c r="G56" s="16">
+        <v>-1</v>
+      </c>
+      <c r="H56" s="16">
+        <v>0</v>
+      </c>
+      <c r="I56" s="11"/>
+      <c r="J56" s="0" t="str">
+        <v>A</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" customFormat="false" ht="30" customHeight="1">
+      <c r="A57" s="6">
+        <v>56</v>
+      </c>
+      <c r="B57" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C57" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="D57" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="E57" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F57" s="16">
+        <v>3</v>
+      </c>
+      <c r="G57" s="16">
+        <v>-1</v>
+      </c>
+      <c r="H57" s="16">
+        <v>0</v>
+      </c>
+      <c r="I57" s="11"/>
+      <c r="J57" s="0" t="str">
+        <v>D</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" customFormat="false" ht="30" customHeight="1">
+      <c r="A58" s="6">
+        <v>57</v>
+      </c>
+      <c r="B58" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C58" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="D58" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="E58" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F58" s="16">
+        <v>3</v>
+      </c>
+      <c r="G58" s="16">
+        <v>-1</v>
+      </c>
+      <c r="H58" s="16">
+        <v>0</v>
+      </c>
+      <c r="I58" s="11"/>
+      <c r="J58" s="0" t="str">
+        <v>D</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" customFormat="false" ht="30" customHeight="1">
+      <c r="A59" s="6">
+        <v>58</v>
+      </c>
+      <c r="B59" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C59" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="D59" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="E59" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F59" s="16">
+        <v>3</v>
+      </c>
+      <c r="G59" s="16">
+        <v>-1</v>
+      </c>
+      <c r="H59" s="16">
+        <v>0</v>
+      </c>
+      <c r="I59" s="11"/>
+      <c r="J59" s="0" t="str">
+        <v>A</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" customFormat="false" ht="30" customHeight="1">
+      <c r="A60" s="6">
+        <v>59</v>
+      </c>
+      <c r="B60" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C60" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="D60" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="E60" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F60" s="16">
+        <v>3</v>
+      </c>
+      <c r="G60" s="16">
+        <v>-1</v>
+      </c>
+      <c r="H60" s="16">
+        <v>0</v>
+      </c>
+      <c r="I60" s="11"/>
+      <c r="J60" s="0" t="str">
+        <v>C</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" customFormat="false" ht="30" customHeight="1">
+      <c r="A61" s="6">
+        <v>60</v>
+      </c>
+      <c r="B61" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C61" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="D61" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="E61" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F61" s="16">
+        <v>3</v>
+      </c>
+      <c r="G61" s="16">
+        <v>-1</v>
+      </c>
+      <c r="H61" s="16">
+        <v>0</v>
+      </c>
+      <c r="I61" s="11"/>
+      <c r="J61" s="0" t="str">
+        <v>C</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" customFormat="false" ht="30" customHeight="1">
+      <c r="A62" s="6">
+        <v>61</v>
+      </c>
+      <c r="B62" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C62" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="D62" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="E62" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F62" s="16">
+        <v>3</v>
+      </c>
+      <c r="G62" s="16">
+        <v>-1</v>
+      </c>
+      <c r="H62" s="16">
+        <v>0</v>
+      </c>
+      <c r="I62" s="11"/>
+      <c r="J62" s="0" t="str">
+        <v>A</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" customFormat="false" ht="30" customHeight="1">
+      <c r="A63" s="6">
+        <v>62</v>
+      </c>
+      <c r="B63" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C63" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="D63" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="E63" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F63" s="16">
+        <v>3</v>
+      </c>
+      <c r="G63" s="16">
+        <v>-1</v>
+      </c>
+      <c r="H63" s="16">
+        <v>0</v>
+      </c>
+      <c r="I63" s="11"/>
+      <c r="J63" s="0" t="str">
+        <v>C</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" customFormat="false" ht="30" customHeight="1">
+      <c r="A64" s="6">
+        <v>63</v>
+      </c>
+      <c r="B64" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C64" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D64" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="E64" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F64" s="16">
+        <v>3</v>
+      </c>
+      <c r="G64" s="16">
+        <v>-1</v>
+      </c>
+      <c r="H64" s="16">
+        <v>0</v>
+      </c>
+      <c r="I64" s="11"/>
+      <c r="J64" s="0" t="str">
+        <v>D</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" customFormat="false" ht="30" customHeight="1">
+      <c r="A65" s="6">
+        <v>64</v>
+      </c>
+      <c r="B65" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C65" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="D65" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="E65" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F65" s="16">
+        <v>3</v>
+      </c>
+      <c r="G65" s="16">
+        <v>-1</v>
+      </c>
+      <c r="H65" s="16">
+        <v>0</v>
+      </c>
+      <c r="I65" s="11"/>
+      <c r="J65" s="0" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" customFormat="false" ht="30" customHeight="1">
+      <c r="A66" s="6">
+        <v>65</v>
+      </c>
+      <c r="B66" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C66" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="D66" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="E66" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F66" s="16">
+        <v>3</v>
+      </c>
+      <c r="G66" s="16">
+        <v>-1</v>
+      </c>
+      <c r="H66" s="16">
+        <v>0</v>
+      </c>
+      <c r="I66" s="11"/>
+      <c r="J66" s="0" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" customFormat="false" ht="30" customHeight="1">
+      <c r="A67" s="6">
+        <v>66</v>
+      </c>
+      <c r="B67" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C67" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="D67" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="E67" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F67" s="16">
+        <v>3</v>
+      </c>
+      <c r="G67" s="16">
+        <v>-1</v>
+      </c>
+      <c r="H67" s="16">
+        <v>0</v>
+      </c>
+      <c r="I67" s="11"/>
+      <c r="J67" s="0" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" customFormat="false" ht="30" customHeight="1">
+      <c r="A68" s="6">
+        <v>67</v>
+      </c>
+      <c r="B68" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C68" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="D68" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="E68" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F68" s="16">
+        <v>3</v>
+      </c>
+      <c r="G68" s="16">
+        <v>-1</v>
+      </c>
+      <c r="H68" s="16">
+        <v>0</v>
+      </c>
+      <c r="I68" s="11"/>
+      <c r="J68" s="0" t="str">
+        <v>D</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" customFormat="false" ht="30" customHeight="1">
+      <c r="A69" s="6">
+        <v>68</v>
+      </c>
+      <c r="B69" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C69" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="D69" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="E69" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F69" s="16">
+        <v>3</v>
+      </c>
+      <c r="G69" s="16">
+        <v>-1</v>
+      </c>
+      <c r="H69" s="16">
+        <v>0</v>
+      </c>
+      <c r="I69" s="11"/>
+      <c r="J69" s="0" t="str">
+        <v>C</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" customFormat="false" ht="30" customHeight="1">
+      <c r="A70" s="6">
+        <v>69</v>
+      </c>
+      <c r="B70" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C70" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="D70" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="E70" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F70" s="16">
+        <v>3</v>
+      </c>
+      <c r="G70" s="16">
+        <v>-1</v>
+      </c>
+      <c r="H70" s="16">
+        <v>0</v>
+      </c>
+      <c r="I70" s="11"/>
+      <c r="J70" s="0" t="str">
+        <v>C</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" customFormat="false" ht="30" customHeight="1">
+      <c r="A71" s="6">
+        <v>70</v>
+      </c>
+      <c r="B71" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C71" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="D71" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="E71" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F71" s="16">
+        <v>3</v>
+      </c>
+      <c r="G71" s="16">
+        <v>-1</v>
+      </c>
+      <c r="H71" s="16">
+        <v>0</v>
+      </c>
+      <c r="I71" s="11"/>
+      <c r="J71" s="0" t="str">
+        <v>D</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" customFormat="false" ht="30" customHeight="1">
+      <c r="A72" s="6">
+        <v>71</v>
+      </c>
+      <c r="B72" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C72" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="D72" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="E72" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F72" s="16">
+        <v>3</v>
+      </c>
+      <c r="G72" s="16">
+        <v>-1</v>
+      </c>
+      <c r="H72" s="16">
+        <v>0</v>
+      </c>
+      <c r="I72" s="11"/>
+      <c r="J72" s="0" t="str">
+        <v>C</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" customFormat="false" ht="30" customHeight="1">
+      <c r="A73" s="6">
+        <v>72</v>
+      </c>
+      <c r="B73" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C73" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="D73" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="E73" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F73" s="16">
+        <v>3</v>
+      </c>
+      <c r="G73" s="16">
+        <v>-1</v>
+      </c>
+      <c r="H73" s="16">
+        <v>0</v>
+      </c>
+      <c r="I73" s="11"/>
+      <c r="J73" s="0" t="str">
+        <v>A</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" customFormat="false" ht="30" customHeight="1">
+      <c r="A74" s="6">
+        <v>73</v>
+      </c>
+      <c r="B74" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C74" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="D74" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="E74" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F74" s="16">
+        <v>3</v>
+      </c>
+      <c r="G74" s="16">
+        <v>-1</v>
+      </c>
+      <c r="H74" s="16">
+        <v>0</v>
+      </c>
+      <c r="I74" s="11"/>
+      <c r="J74" s="0" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" customFormat="false" ht="30" customHeight="1">
+      <c r="A75" s="6">
+        <v>74</v>
+      </c>
+      <c r="B75" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C75" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="D75" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="E75" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F75" s="16">
+        <v>3</v>
+      </c>
+      <c r="G75" s="16">
+        <v>-1</v>
+      </c>
+      <c r="H75" s="16">
+        <v>0</v>
+      </c>
+      <c r="I75" s="11"/>
+      <c r="J75" s="0" t="str">
+        <v>D</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" customFormat="false" ht="30" customHeight="1">
+      <c r="A76" s="6">
+        <v>75</v>
+      </c>
+      <c r="B76" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C76" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D76" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="E76" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F76" s="16">
+        <v>3</v>
+      </c>
+      <c r="G76" s="16">
+        <v>-1</v>
+      </c>
+      <c r="H76" s="16">
+        <v>0</v>
+      </c>
+      <c r="I76" s="11"/>
+      <c r="J76" s="0" t="str">
+        <v>A</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" customFormat="false" ht="30" customHeight="1">
+      <c r="A77" s="6">
+        <v>76</v>
+      </c>
+      <c r="B77" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C77" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="D77" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="E77" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F77" s="16">
+        <v>3</v>
+      </c>
+      <c r="G77" s="16">
+        <v>-1</v>
+      </c>
+      <c r="H77" s="16">
+        <v>0</v>
+      </c>
+      <c r="I77" s="11"/>
+      <c r="J77" s="0" t="str">
+        <v>D</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" customFormat="false" ht="30" customHeight="1">
+      <c r="A78" s="6">
+        <v>77</v>
+      </c>
+      <c r="B78" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C78" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="D78" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="E78" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F78" s="16">
+        <v>3</v>
+      </c>
+      <c r="G78" s="16">
+        <v>-1</v>
+      </c>
+      <c r="H78" s="16">
+        <v>0</v>
+      </c>
+      <c r="I78" s="11"/>
+      <c r="J78" s="0" t="str">
+        <v>C</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" customFormat="false" ht="30" customHeight="1">
+      <c r="A79" s="6">
+        <v>78</v>
+      </c>
+      <c r="B79" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C79" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="D79" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="E79" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F79" s="16">
+        <v>3</v>
+      </c>
+      <c r="G79" s="16">
+        <v>-1</v>
+      </c>
+      <c r="H79" s="16">
+        <v>0</v>
+      </c>
+      <c r="I79" s="11"/>
+      <c r="J79" s="0" t="str">
+        <v>A</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" customFormat="false" ht="30" customHeight="1">
+      <c r="A80" s="6">
+        <v>79</v>
+      </c>
+      <c r="B80" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C80" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="D80" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="E80" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F80" s="16">
+        <v>3</v>
+      </c>
+      <c r="G80" s="16">
+        <v>-1</v>
+      </c>
+      <c r="H80" s="16">
+        <v>0</v>
+      </c>
+      <c r="I80" s="11"/>
+      <c r="J80" s="0" t="str">
+        <v>C</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" customFormat="false" ht="30" customHeight="1">
+      <c r="A81" s="6">
+        <v>80</v>
+      </c>
+      <c r="B81" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C81" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="D81" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="E81" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F81" s="16">
+        <v>3</v>
+      </c>
+      <c r="G81" s="16">
+        <v>-1</v>
+      </c>
+      <c r="H81" s="16">
+        <v>0</v>
+      </c>
+      <c r="I81" s="11"/>
+      <c r="J81" s="0" t="str">
+        <v>A</v>
       </c>
     </row>
   </sheetData>

</xml_diff>